<commit_message>
Added servers + UIDs from graph db
</commit_message>
<xml_diff>
--- a/data/in/MiddlewareConfigTableDefinition.xlsx
+++ b/data/in/MiddlewareConfigTableDefinition.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="95">
   <si>
     <t>mftType</t>
   </si>
@@ -132,8 +132,8 @@
     <t>L3Y-PROD-CH/WM</t>
   </si>
   <si>
-    <t>1946
-2686</t>
+    <t>a1946
+a2686</t>
   </si>
   <si>
     <t>(001,P0)
@@ -143,8 +143,8 @@
     <t>L3Y-PROD-DE/IT/HK/SG</t>
   </si>
   <si>
-    <t>2020
-4230</t>
+    <t>a2020
+a4230</t>
   </si>
   <si>
     <t>(891,P7)
@@ -154,8 +154,8 @@
     <t>L3Y-TE2-CH/WM</t>
   </si>
   <si>
-    <t>2222
-3333</t>
+    <t>a2222
+a3333</t>
   </si>
   <si>
     <t>(001,R0)
@@ -165,8 +165,8 @@
     <t>L3Y-TE2-DE/IT/HK/SG</t>
   </si>
   <si>
-    <t>4444
-5555</t>
+    <t>a4444
+a5555</t>
   </si>
   <si>
     <t>(891,R7)
@@ -176,8 +176,8 @@
     <t>L3Y-TE1</t>
   </si>
   <si>
-    <t>5059
-2002</t>
+    <t>a5059
+a2002</t>
   </si>
   <si>
     <t>(001,I0)
@@ -185,8 +185,7 @@
   </si>
   <si>
     <t>swComponent
-mftType
-serverGroup</t>
+mftType</t>
   </si>
   <si>
     <t>postScript</t>
@@ -213,115 +212,112 @@
     <t>op l3xltapp post</t>
   </si>
   <si>
+    <t>op l3xltapp post ibc</t>
+  </si>
+  <si>
+    <t>op l3xltapp post prc</t>
+  </si>
+  <si>
+    <t>postScriptParams</t>
+  </si>
+  <si>
+    <t>hasPostScriptParams</t>
+  </si>
+  <si>
+    <t>rx\:DEMAN ($EF1031)? $FG</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>$DEMAN $EF1031 $FG</t>
+  </si>
+  <si>
+    <t>019;891;898;890;895</t>
+  </si>
+  <si>
+    <t>FA8;FB8</t>
+  </si>
+  <si>
+    <t>DEMAN=DEMAN EF1031=$EF1031 FG=$FG $FOW</t>
+  </si>
+  <si>
+    <t>receiverDirectory</t>
+  </si>
+  <si>
+    <t>hasReceiverDirectory</t>
+  </si>
+  <si>
+    <t>/app/L3X/dyn/asi</t>
+  </si>
+  <si>
+    <t>/app/FA8/dyn/asi</t>
+  </si>
+  <si>
+    <t>/app/FB8/dyn/asi</t>
+  </si>
+  <si>
+    <t>UID</t>
+  </si>
+  <si>
+    <t>hasUID</t>
+  </si>
+  <si>
+    <t>L3Y;L3Z</t>
+  </si>
+  <si>
+    <t>ul3y1001</t>
+  </si>
+  <si>
+    <t>ufa81001</t>
+  </si>
+  <si>
+    <t>ufb81001</t>
+  </si>
+  <si>
+    <t>hasSender</t>
+  </si>
+  <si>
+    <t>hasReceiver</t>
+  </si>
+  <si>
+    <t>(891,P7)-&gt;(891,P7)</t>
+  </si>
+  <si>
+    <t>(891,P7)</t>
+  </si>
+  <si>
+    <t>(898,P2)-&gt;(898,P2)</t>
+  </si>
+  <si>
+    <t>(898,P2)</t>
+  </si>
+  <si>
+    <t>(890,P8)-&gt;(890,P8)</t>
+  </si>
+  <si>
+    <t>(890,P8)</t>
+  </si>
+  <si>
+    <t>019</t>
+  </si>
+  <si>
+    <t>P7</t>
+  </si>
+  <si>
+    <t>P0</t>
+  </si>
+  <si>
+    <t>891</t>
+  </si>
+  <si>
+    <t>898</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
     <t>890</t>
-  </si>
-  <si>
-    <t>P7;P8</t>
-  </si>
-  <si>
-    <t>op l3xltapp post ibc</t>
-  </si>
-  <si>
-    <t>op l3xltapp post prc</t>
-  </si>
-  <si>
-    <t>postScriptParams</t>
-  </si>
-  <si>
-    <t>hasPostScriptParams</t>
-  </si>
-  <si>
-    <t>rx\:DEMAN ($EF1031)? $FG</t>
-  </si>
-  <si>
-    <t>001</t>
-  </si>
-  <si>
-    <t>$DEMAN $EF1031 $FG</t>
-  </si>
-  <si>
-    <t>019;891;898;890;895</t>
-  </si>
-  <si>
-    <t>FA8;FB8</t>
-  </si>
-  <si>
-    <t>DEMAN=DEMAN EF1031=$EF1031 FG=$FG $FOW</t>
-  </si>
-  <si>
-    <t>receiverDirectory</t>
-  </si>
-  <si>
-    <t>hasReceiverDirectory</t>
-  </si>
-  <si>
-    <t>/app/L3X/dyn/asi</t>
-  </si>
-  <si>
-    <t>/app/FA8/dyn/asi</t>
-  </si>
-  <si>
-    <t>/app/FB8/dyn/asi</t>
-  </si>
-  <si>
-    <t>UID</t>
-  </si>
-  <si>
-    <t>hasUID</t>
-  </si>
-  <si>
-    <t>L3Y;L3Z</t>
-  </si>
-  <si>
-    <t>ul3y1001</t>
-  </si>
-  <si>
-    <t>ufa81001</t>
-  </si>
-  <si>
-    <t>ufb81001</t>
-  </si>
-  <si>
-    <t>hasSender</t>
-  </si>
-  <si>
-    <t>hasReceiver</t>
-  </si>
-  <si>
-    <t>(891,P7)-&gt;(891,P7)</t>
-  </si>
-  <si>
-    <t>(891,P7)</t>
-  </si>
-  <si>
-    <t>(898,P2)-&gt;(898,P2)</t>
-  </si>
-  <si>
-    <t>(898,P2)</t>
-  </si>
-  <si>
-    <t>(890,P8)-&gt;(890,P8)</t>
-  </si>
-  <si>
-    <t>(890,P8)</t>
-  </si>
-  <si>
-    <t>019</t>
-  </si>
-  <si>
-    <t>P7</t>
-  </si>
-  <si>
-    <t>P0</t>
-  </si>
-  <si>
-    <t>891</t>
-  </si>
-  <si>
-    <t>898</t>
-  </si>
-  <si>
-    <t>P2</t>
   </si>
   <si>
     <t>P8</t>
@@ -393,7 +389,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -418,11 +414,11 @@
     <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf quotePrefix="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf quotePrefix="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -435,6 +431,9 @@
     </xf>
     <xf borderId="0" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf quotePrefix="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -884,7 +883,7 @@
       <c r="B3" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="D3" s="5" t="s">
@@ -898,7 +897,7 @@
       <c r="B4" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="8" t="s">
         <v>38</v>
       </c>
       <c r="D4" s="5" t="s">
@@ -912,7 +911,7 @@
       <c r="B5" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="8" t="s">
         <v>41</v>
       </c>
       <c r="D5" s="5" t="s">
@@ -926,7 +925,7 @@
       <c r="B6" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="8" t="s">
         <v>44</v>
       </c>
       <c r="D6" s="5" t="s">
@@ -940,7 +939,7 @@
       <c r="B7" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="8" t="s">
         <v>47</v>
       </c>
       <c r="D7" s="5" t="s">
@@ -969,7 +968,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="9" t="s">
         <v>49</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1007,19 +1006,13 @@
       <c r="B3" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5">
@@ -1027,7 +1020,7 @@
         <v>25</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1053,11 +1046,11 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="9" t="s">
         <v>49</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>51</v>
@@ -1071,7 +1064,7 @@
     </row>
     <row r="2">
       <c r="A2" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="4" t="s">
@@ -1089,29 +1082,29 @@
         <v>9</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C4" s="5" t="s">
         <v>65</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1137,11 +1130,11 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="9" t="s">
         <v>49</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>51</v>
@@ -1155,7 +1148,7 @@
     </row>
     <row r="2">
       <c r="A2" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="4" t="s">
@@ -1173,23 +1166,23 @@
         <v>9</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>72</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1213,11 +1206,11 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="6" t="s">
-        <v>49</v>
+      <c r="A1" s="9" t="s">
+        <v>1</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>51</v>
@@ -1231,7 +1224,7 @@
     </row>
     <row r="2">
       <c r="A2" s="12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="4" t="s">
@@ -1245,11 +1238,11 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="9" t="s">
-        <v>77</v>
+      <c r="A3" s="8" t="s">
+        <v>75</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4">
@@ -1257,7 +1250,7 @@
         <v>23</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5">
@@ -1265,7 +1258,7 @@
         <v>29</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1302,10 +1295,10 @@
     <row r="2">
       <c r="A2" s="3"/>
       <c r="B2" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3">
@@ -1332,35 +1325,35 @@
     </row>
     <row r="5">
       <c r="A5" s="13" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="13" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1403,10 +1396,10 @@
         <v>13</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4">
@@ -1414,43 +1407,43 @@
         <v>12</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="13" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="13" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>58</v>
+        <v>86</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>93</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>